<commit_message>
Update file permissions for opportunity templates
</commit_message>
<xml_diff>
--- a/data_model_upload_template/employer_opportunities_template.xlsx
+++ b/data_model_upload_template/employer_opportunities_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\arman\uni\y3\sem2\CS3528\data_model_upload_template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB9FA35D-538D-4F85-833E-E1F525CC1D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A78A2E3-116E-4E3E-B1F4-D76CF71433F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="49">
   <si>
     <t>Title</t>
   </si>
@@ -136,6 +136,42 @@
   </si>
   <si>
     <t>12_months</t>
+  </si>
+  <si>
+    <t>Location</t>
+  </si>
+  <si>
+    <t>123 Dummy road</t>
+  </si>
+  <si>
+    <t>124 Dummy road</t>
+  </si>
+  <si>
+    <t>125 Dummy road</t>
+  </si>
+  <si>
+    <t>126 Dummy road</t>
+  </si>
+  <si>
+    <t>127 Dummy road</t>
+  </si>
+  <si>
+    <t>128 Dummy road</t>
+  </si>
+  <si>
+    <t>129 Dummy road</t>
+  </si>
+  <si>
+    <t>130 Dummy road</t>
+  </si>
+  <si>
+    <t>131 Dummy road</t>
+  </si>
+  <si>
+    <t>132 Dummy road</t>
+  </si>
+  <si>
+    <t>133 Dummy road</t>
   </si>
 </sst>
 </file>
@@ -459,24 +495,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G12"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D1048576"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="4.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -487,19 +524,22 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -510,19 +550,22 @@
         <v>8</v>
       </c>
       <c r="D2" t="s">
+        <v>38</v>
+      </c>
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>6</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -533,19 +576,22 @@
         <v>8</v>
       </c>
       <c r="D3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" t="s">
         <v>11</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>12</v>
       </c>
-      <c r="F3">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="G3">
+        <v>7</v>
+      </c>
+      <c r="H3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -556,19 +602,22 @@
         <v>8</v>
       </c>
       <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
         <v>13</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>14</v>
       </c>
-      <c r="F4">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -579,19 +628,22 @@
         <v>8</v>
       </c>
       <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
         <v>15</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>16</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>9</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>7</v>
       </c>
@@ -602,19 +654,22 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
         <v>17</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>18</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>10</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -625,19 +680,22 @@
         <v>8</v>
       </c>
       <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>20</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>11</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -648,19 +706,22 @@
         <v>8</v>
       </c>
       <c r="D8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" t="s">
         <v>21</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>22</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>12</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -671,19 +732,22 @@
         <v>8</v>
       </c>
       <c r="D9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E9" t="s">
         <v>23</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>24</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>13</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -694,19 +758,22 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
+        <v>46</v>
+      </c>
+      <c r="E10" t="s">
         <v>25</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>26</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>14</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -717,19 +784,22 @@
         <v>8</v>
       </c>
       <c r="D11" t="s">
+        <v>47</v>
+      </c>
+      <c r="E11" t="s">
         <v>27</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>28</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>15</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -740,15 +810,18 @@
         <v>8</v>
       </c>
       <c r="D12" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" t="s">
         <v>29</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>30</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>16</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>